<commit_message>
importar usuarios clientes, notficiaciones
</commit_message>
<xml_diff>
--- a/public/archivos/clientes.xlsx
+++ b/public/archivos/clientes.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11013"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juanmoscoso/Proyectos/CRM/CRM_web/public/archivos/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3A43087-413C-3C48-9D97-340D0A0486EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40240" yWindow="0" windowWidth="30880" windowHeight="18380" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14700" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140000"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="51">
   <si>
     <t>Empresa</t>
   </si>
@@ -124,12 +130,60 @@
   </si>
   <si>
     <t>sd</t>
+  </si>
+  <si>
+    <t>vendedor_cedula</t>
+  </si>
+  <si>
+    <t>vendedor_nombre</t>
+  </si>
+  <si>
+    <t>vendedor_apellido</t>
+  </si>
+  <si>
+    <t>vendedor_email</t>
+  </si>
+  <si>
+    <t>09090900</t>
+  </si>
+  <si>
+    <t>Juan</t>
+  </si>
+  <si>
+    <t>Perez</t>
+  </si>
+  <si>
+    <t>perez@crm.com</t>
+  </si>
+  <si>
+    <t>Claudio</t>
+  </si>
+  <si>
+    <t>Loja</t>
+  </si>
+  <si>
+    <t>juan.moscoso@primme.tech</t>
+  </si>
+  <si>
+    <t>0103902399432</t>
+  </si>
+  <si>
+    <t>0090902392</t>
+  </si>
+  <si>
+    <t>algo</t>
+  </si>
+  <si>
+    <t>nuevo</t>
+  </si>
+  <si>
+    <t>nuevo@otro.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -172,21 +226,33 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="3" builtinId="8"/>
     <cellStyle name="Hipervínculo visitado" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -511,14 +577,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:R4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="9" max="9" width="17.5" customWidth="1"/>
     <col min="10" max="10" width="15.1640625" customWidth="1"/>
@@ -526,9 +592,10 @@
     <col min="12" max="12" width="16.33203125" customWidth="1"/>
     <col min="13" max="13" width="18.1640625" customWidth="1"/>
     <col min="14" max="14" width="14.1640625" customWidth="1"/>
+    <col min="15" max="15" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -571,8 +638,20 @@
       <c r="N1" t="s">
         <v>11</v>
       </c>
+      <c r="O1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="P1" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>37</v>
+      </c>
+      <c r="R1" t="s">
+        <v>38</v>
+      </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -609,8 +688,20 @@
       <c r="L2" t="s">
         <v>32</v>
       </c>
+      <c r="O2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="P2" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>41</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>42</v>
+      </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -647,8 +738,20 @@
       <c r="L3" t="s">
         <v>33</v>
       </c>
+      <c r="O3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="P3" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>44</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>45</v>
+      </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -685,8 +788,25 @@
       <c r="L4" t="s">
         <v>34</v>
       </c>
+      <c r="O4" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="P4" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>49</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="R2" r:id="rId1" xr:uid="{9A75F40E-043C-C049-B5E9-A8EBEA8E087C}"/>
+    <hyperlink ref="R3" r:id="rId2" xr:uid="{EE5FB531-E301-994E-B347-F16543B92EB4}"/>
+    <hyperlink ref="R4" r:id="rId3" xr:uid="{BE591CB9-355E-C042-88CC-F7DC489E3F9B}"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>